<commit_message>
Strukturanpassung und Weinkarte aktualisiert
</commit_message>
<xml_diff>
--- a/weine.xlsx
+++ b/weine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\winecard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\enoteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D52F830-645C-44FE-AF48-E27E98EEA9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8951C2-85AA-4859-8015-361FBABA34A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="3660" windowWidth="16200" windowHeight="9015" xr2:uid="{DC1CDB42-73D2-46F4-A222-166C1E15EEE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC1CDB42-73D2-46F4-A222-166C1E15EEE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
   <si>
     <t>Weingut</t>
   </si>
@@ -75,18 +75,6 @@
     <t>Germania</t>
   </si>
   <si>
-    <t>Augustiner Hell</t>
-  </si>
-  <si>
-    <t>Grüner Silvaner trocken</t>
-  </si>
-  <si>
-    <t>Mineralgestein Riesling trocken</t>
-  </si>
-  <si>
-    <t>Weissburgunder Löss trocken</t>
-  </si>
-  <si>
     <t>Wohlmuth</t>
   </si>
   <si>
@@ -96,12 +84,6 @@
     <t>Österreich</t>
   </si>
   <si>
-    <t>Sauvignon Blanc trocken</t>
-  </si>
-  <si>
-    <t>Sileni</t>
-  </si>
-  <si>
     <t>Marlborough</t>
   </si>
   <si>
@@ -111,28 +93,109 @@
     <t>Fattoria La Vialla</t>
   </si>
   <si>
-    <t>Sangiovese Cabernet Sauvignon Barriccato</t>
-  </si>
-  <si>
-    <t>Vernaccia Riserva trocken</t>
-  </si>
-  <si>
-    <t>Weißwein</t>
-  </si>
-  <si>
-    <t>Rotwein</t>
-  </si>
-  <si>
     <t>Helles</t>
   </si>
   <si>
     <t>Weißbier</t>
   </si>
   <si>
-    <t>Schneider TAP7</t>
-  </si>
-  <si>
     <t>Art</t>
+  </si>
+  <si>
+    <t>Aktiv</t>
+  </si>
+  <si>
+    <t>Rebsorten</t>
+  </si>
+  <si>
+    <t>Cortona Syrah Riserva</t>
+  </si>
+  <si>
+    <t>Syrah</t>
+  </si>
+  <si>
+    <t>Barriccato</t>
+  </si>
+  <si>
+    <t>Sangiovese, Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon, Merlot</t>
+  </si>
+  <si>
+    <t>Vernaccia di San Gimignano Riserva trocken</t>
+  </si>
+  <si>
+    <t>Sauvignon Blanc</t>
+  </si>
+  <si>
+    <t>Augustiner</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Grüner Silvaner</t>
+  </si>
+  <si>
+    <t>SeccioMoro (non filtrato)</t>
+  </si>
+  <si>
+    <t>Casal Duro (non filtrato)</t>
+  </si>
+  <si>
+    <t>u.a. Sangiovese</t>
+  </si>
+  <si>
+    <t>Grauburgunder</t>
+  </si>
+  <si>
+    <t>Blanc de Noir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mineralgestein Riesling </t>
+  </si>
+  <si>
+    <t>Weissburgunder Löss</t>
+  </si>
+  <si>
+    <t>Spätburgunder</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
+    <t>Frankreich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap sur l'Atlantique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauvignon Blanc </t>
+  </si>
+  <si>
+    <t>Sileni Cellar Selection</t>
+  </si>
+  <si>
+    <t>Franziskaner</t>
+  </si>
+  <si>
+    <t>Atlantique</t>
+  </si>
+  <si>
+    <t>Weltenburger</t>
+  </si>
+  <si>
+    <t>Weißbier TAP7</t>
+  </si>
+  <si>
+    <t>Anno 1050</t>
+  </si>
+  <si>
+    <t>Vino Bianco</t>
+  </si>
+  <si>
+    <t>Vino Rosso</t>
   </si>
 </sst>
 </file>
@@ -498,18 +561,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99428D0-AF9E-44C8-A611-98D6922EEEE3}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="28.9296875" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,16 +589,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -540,16 +615,20 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>2024</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -560,16 +639,20 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>2024</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -580,118 +663,146 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>2024</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>2024</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2024</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2022</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>2023</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>2023</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -700,53 +811,342 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2023</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G17" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="G19" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2">
+        <v>2025</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
         <v>2025</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2">
+        <v>2025</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2">
         <v>2025</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>